<commit_message>
fix format file Excel, and import excel
</commit_message>
<xml_diff>
--- a/DATH/TestFirst.xlsx
+++ b/DATH/TestFirst.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aab93733cffe055c/Tài liệu trên lớp/DATH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="14_{81D13E2D-C283-4DE3-B4D4-16203839DE98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9B8AC88-849E-47FD-B91A-9FE40E6EA6C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B511DCEB-FE43-4D06-A910-DC6103CD129B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{053C4792-58B4-47A6-9971-A22CA7A92AB0}"/>
   </bookViews>
@@ -31,7 +31,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+  <si>
+    <t>UniqueId</t>
+  </si>
   <si>
     <t>ProjectTypeId</t>
   </si>
@@ -42,19 +45,34 @@
     <t>Description</t>
   </si>
   <si>
-    <t>StudentCode1</t>
-  </si>
-  <si>
-    <t>StudentCode2</t>
-  </si>
-  <si>
-    <t>StudentCode3</t>
-  </si>
-  <si>
-    <t>LecturerCode1</t>
-  </si>
-  <si>
-    <t>LecturerCode2</t>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>StudentCode</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>LecturerCode</t>
+  </si>
+  <si>
+    <t>Weeks</t>
+  </si>
+  <si>
+    <t>a1b2c08c-7dbd-468c-94b8-75006c033845</t>
   </si>
   <si>
     <t>Hệ thống quản lý đồ án sinh viên</t>
@@ -63,35 +81,98 @@
     <t>Mô tả</t>
   </si>
   <si>
+    <t>16DTHC2</t>
+  </si>
+  <si>
+    <t>Đặng Minh</t>
+  </si>
+  <si>
+    <t>Đạt</t>
+  </si>
+  <si>
+    <t>dmdattadmd@gmail.com</t>
+  </si>
+  <si>
     <t>nguyenmanhhung</t>
   </si>
   <si>
+    <t>Nguyễn Mạnh</t>
+  </si>
+  <si>
+    <t>Hùng</t>
+  </si>
+  <si>
+    <t>thayhung@email.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng</t>
+  </si>
+  <si>
+    <t>Nhật</t>
+  </si>
+  <si>
+    <t>e1c614e8-52cb-4434-886c-178c61f8ca8a</t>
+  </si>
+  <si>
     <t>Web bán thiết bị an ninh</t>
   </si>
   <si>
     <t>Làm bằng python và mongodb</t>
   </si>
   <si>
-    <t>UniqueId</t>
-  </si>
-  <si>
-    <t>a1b2c08c-7dbd-468c-94b8-75006c033845</t>
-  </si>
-  <si>
-    <t>e1c614e8-52cb-4434-886c-178c61f8ca8a</t>
-  </si>
-  <si>
-    <t>Weeks</t>
+    <t>16DTHB3</t>
+  </si>
+  <si>
+    <t>Phạm Minh</t>
+  </si>
+  <si>
+    <t>Khiêm</t>
+  </si>
+  <si>
+    <t>14d25a17-4573-408c-98ca-be82e1986eec</t>
+  </si>
+  <si>
+    <t>He thong tào lao</t>
+  </si>
+  <si>
+    <t>bai thông</t>
+  </si>
+  <si>
+    <t>16DTHB52</t>
+  </si>
+  <si>
+    <t>minhdat@gmail.com</t>
+  </si>
+  <si>
+    <t>dangminhdat</t>
+  </si>
+  <si>
+    <t>thaydat@email.com</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>0798059927</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -115,14 +196,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,114 +529,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469FD84D-4B99-4459-9CB1-615E9936D584}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.875" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" customWidth="1"/>
+    <col min="17" max="17" width="21.875" customWidth="1"/>
+    <col min="19" max="19" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1611061191</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
+        <v>1611062192</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1611061191</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="3">
+        <v>1</v>
+      </c>
+      <c r="S4" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
+        <v>1611062192</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
+        <v>1611060417</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1611061191</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1611062192</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1911060417</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="3">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
         <v>12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1611061191</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1611062192</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1611060417</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{B074C63B-01B6-42AF-A148-E70E884F5784}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{CD8859EE-3C64-466E-9C70-3B6E00F3E97C}"/>
+    <hyperlink ref="P2" r:id="rId3" xr:uid="{9C344B45-C85F-4AFF-B066-59E5BE6330A5}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{1C92FDF5-335A-46B6-98D9-DA1B19ECBAF4}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{DE058D61-D5E3-464C-A997-D2795D228FEC}"/>
+    <hyperlink ref="P7" r:id="rId6" xr:uid="{1554F7B6-A72F-4BEE-8271-C719BBCCCA27}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>